<commit_message>
Added Bid and fixed class relationships
</commit_message>
<xml_diff>
--- a/appdev_project2/doc/db.xlsx
+++ b/appdev_project2/doc/db.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumenty\Eclipse\appdev_project2\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumenty\College\Year 4\App Dev Frameworks\Project2\appdev_project2\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{4B8CF8AE-96B7-49AE-BD08-879708C36338}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27A2351-35CE-4F23-90B8-12D19D89EA9C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CC068F78-8EF7-4910-A6CC-A0B4719ED0EE}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{CC068F78-8EF7-4910-A6CC-A0B4719ED0EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="49">
   <si>
     <t>User</t>
   </si>
@@ -159,9 +159,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>JobOwners</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>bidValue (€)</t>
+  </si>
+  <si>
+    <t>owner</t>
   </si>
 </sst>
 </file>
@@ -250,7 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -266,6 +266,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -581,10 +582,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5113A91-4522-4414-898B-65952C637622}">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +595,7 @@
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
     <col min="5" max="5" width="21.140625" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -621,13 +622,13 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -719,19 +720,23 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
         <v>46</v>
       </c>
-      <c r="F9" t="s">
-        <v>47</v>
+      <c r="G9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -747,6 +752,9 @@
       <c r="F10" s="4">
         <v>43775</v>
       </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -761,6 +769,9 @@
       <c r="F11" s="4">
         <v>43770</v>
       </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -775,6 +786,9 @@
       <c r="F12" s="4">
         <v>43772</v>
       </c>
+      <c r="G12" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -789,202 +803,159 @@
       <c r="F13" s="4">
         <v>43774</v>
       </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="B16" t="s">
-        <v>3</v>
+      <c r="C16" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C17" s="3">
+        <v>150</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
+      <c r="C18" s="3">
+        <v>200</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C19" s="3">
+        <v>500</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="3">
+        <v>250</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="3">
+        <v>1000</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" t="s">
-        <v>48</v>
-      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="3">
+        <v>550</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="3">
-        <v>150</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="A24" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="6"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="3">
-        <v>200</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="3">
-        <v>500</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+        <v>36</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="3">
-        <v>250</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+        <v>36</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="3">
-        <v>1000</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+        <v>36</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="3">
-        <v>550</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="6"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>11</v>
-      </c>
-      <c r="B34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>37</v>
       </c>
-      <c r="B36" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="B30" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>